<commit_message>
Feature: Add joint borrowers support to Excel import with enterprise test data
</commit_message>
<xml_diff>
--- a/贷款到期清单.xlsx
+++ b/贷款到期清单.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:AC7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,75 +476,105 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
+          <t>共同借款人1名称</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>共同借款人1证件号</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>共同借款人1联系方式</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>共同借款人2名称</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>共同借款人2证件号</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>共同借款人2联系方式</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>担保人1名称</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>担保人1身份证</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>担保人1联系方式</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>担保人2名称</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>担保人2身份证</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>担保人2联系方式</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>担保人3名称</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>担保人3身份证</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>担保人3联系方式</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>担保人4名称</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>担保人4身份证</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>担保人4联系方式</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>担保人5名称</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>担保人5身份证</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>担保人5联系方式</t>
         </is>
@@ -593,43 +623,61 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>赵强</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>330107198406061111</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>13700137011</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>刘强</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>330106198306061111</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>13700137001</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>郑丽</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>330110198409095555</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>13600136001</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
-      <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -672,33 +720,51 @@
           <t>13900139002</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>黄丽</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>330110198509092222</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>13600136011</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>孙明</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>330107198508082222</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>13700137002</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -708,22 +774,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>王五</t>
+          <t>王五科技有限公司</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>330104199208203456</t>
+          <t>91330100MA2ABCDE12</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>13800138003</t>
+          <t>0571-88888888</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>杭州市西湖区ZZ巷ZZ号</t>
+          <t>杭州市西湖区科技园A座</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -731,43 +797,61 @@
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
+          <t>杭州云端科技</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>91330100MA2KLMNO56</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0571-77777777</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr">
+        <is>
           <t>周华</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>330108199010103333</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>13700137003</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>冯伟</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>330111199111116666</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>13600136003</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -812,31 +896,247 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>吴刚</t>
+          <t>孙伟</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>330109198212124444</t>
+          <t>330108199211112222</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>13700137004</t>
+          <t>13700137012</t>
         </is>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>吴刚</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>330109198212124444</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>13700137004</t>
+        </is>
+      </c>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>拱墅支行</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>钱七实业集团</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>91330100MA2FGHIJ34</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0571-99999999</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>杭州市拱墅区工业路100号</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>李明</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>330109198512123333</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>13700137013</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>上海贸易有限公司</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>91310000MA2PQRST78</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>021-55555555</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>郑伟</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>330110198312125555</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>13700137005</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>杭州融资担保公司</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>91330100MA2UVWXY90</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>0571-66666666</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr"/>
+      <c r="AB6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>余杭支行</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>孙八</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>330106198808083456</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>13800138006</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>杭州市余杭区BB街BB号</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>周婷</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>330106198909094567</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>13900139006</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>吴洁</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>330111199012123333</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>13600136013</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>徐敏</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>330111198411116666</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>13700137006</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>马强</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>330112198601017777</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>13600136006</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
+      <c r="AB7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Feature: Auto-detect and fill enterprise/personal type with joint borrowers support
</commit_message>
<xml_diff>
--- a/贷款到期清单.xlsx
+++ b/贷款到期清单.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC7"/>
+  <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,145 +436,150 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>客户主体</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>支行简称</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>贷款人</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>证件号（对公情况）</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>联系方式（对公情况）</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>住址</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>配偶名</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>身份证</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>联系方式</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>共同借款人1名称</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>共同借款人1证件号</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>共同借款人1联系方式</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>共同借款人2名称</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>共同借款人2证件号</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>共同借款人2联系方式</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>担保人1名称</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>担保人1身份证</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>担保人1联系方式</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>担保人2名称</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>担保人2身份证</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>担保人2联系方式</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>担保人3名称</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>担保人3身份证</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>担保人3联系方式</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>担保人4名称</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>担保人4身份证</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>担保人4联系方式</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>担保人5名称</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>担保人5身份证</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>担保人5联系方式</t>
         </is>
@@ -583,93 +588,97 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>personal</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>城东支行</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>张三</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>330102199001011234</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>13800138001</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>杭州市上城区XX街道XX号</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>王芳</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>330102199105052345</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>13900139001</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>赵强</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>330107198406061111</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>13700137011</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr">
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
         <is>
           <t>刘强</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>330106198306061111</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>13700137001</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="S2" t="inlineStr">
         <is>
           <t>郑丽</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>330110198409095555</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>13600136001</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -678,82 +687,87 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>personal</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>滨江支行</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>李四</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>330103198502152345</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>13800138002</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>杭州市滨江区YY路YY号</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>陈静</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>330103198707083456</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>13900139002</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr">
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
         <is>
           <t>黄丽</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>330110198509092222</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="O3" t="inlineStr">
         <is>
           <t>13600136011</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="P3" t="inlineStr">
         <is>
           <t>孙明</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="Q3" t="inlineStr">
         <is>
           <t>330107198508082222</t>
         </is>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>13700137002</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
@@ -765,85 +779,90 @@
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
       <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>enterprise</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>西湖支行</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>王五科技有限公司</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>91330100MA2ABCDE12</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>0571-88888888</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>杭州市西湖区科技园A座</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr">
         <is>
           <t>杭州云端科技</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>91330100MA2KLMNO56</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>0571-77777777</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
         <is>
           <t>周华</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>330108199010103333</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="R4" t="inlineStr">
         <is>
           <t>13700137003</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" t="inlineStr">
         <is>
           <t>冯伟</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="T4" t="inlineStr">
         <is>
           <t>330111199111116666</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>13600136003</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
@@ -852,82 +871,87 @@
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
       <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>personal</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>萧山支行</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>赵六</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>330105199112124567</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>13800138004</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>杭州市萧山区AA大道AA号</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>钱美丽</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>330105199206154567</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>13900139004</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>孙伟</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>330108199211112222</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>13700137012</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr">
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr">
         <is>
           <t>吴刚</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>330109198212124444</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="R5" t="inlineStr">
         <is>
           <t>13700137004</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
@@ -939,97 +963,102 @@
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
       <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>enterprise</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>拱墅支行</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>钱七实业集团</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>91330100MA2FGHIJ34</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>0571-99999999</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>杭州市拱墅区工业路100号</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr">
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr">
         <is>
           <t>李明</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>330109198512123333</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>13700137013</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>上海贸易有限公司</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>91310000MA2PQRST78</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>021-55555555</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>郑伟</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t>330110198312125555</t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="R6" t="inlineStr">
         <is>
           <t>13700137005</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="S6" t="inlineStr">
         <is>
           <t>杭州融资担保公司</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="T6" t="inlineStr">
         <is>
           <t>91330100MA2UVWXY90</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="U6" t="inlineStr">
         <is>
           <t>0571-66666666</t>
         </is>
       </c>
-      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
@@ -1038,97 +1067,102 @@
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
       <c r="AC6" t="inlineStr"/>
+      <c r="AD6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>personal</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>余杭支行</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>孙八</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>330106198808083456</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>13800138006</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>杭州市余杭区BB街BB号</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>周婷</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>330106198909094567</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>13900139006</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
         <is>
           <t>吴洁</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>330111199012123333</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="O7" t="inlineStr">
         <is>
           <t>13600136013</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="P7" t="inlineStr">
         <is>
           <t>徐敏</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="Q7" t="inlineStr">
         <is>
           <t>330111198411116666</t>
         </is>
       </c>
-      <c r="Q7" t="inlineStr">
+      <c r="R7" t="inlineStr">
         <is>
           <t>13700137006</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="S7" t="inlineStr">
         <is>
           <t>马强</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="T7" t="inlineStr">
         <is>
           <t>330112198601017777</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="U7" t="inlineStr">
         <is>
           <t>13600136006</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
@@ -1137,6 +1171,7 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
+      <c r="AD7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>